<commit_message>
Added a way to put back the kra image that's been dropped
To put back the image, I need the png version of it
since the wmf version is being dropped.
I have also downloaded the package pillow and inserted the image using
openpyxl. It is actually quite easy.
</commit_message>
<xml_diff>
--- a/static/p9.xlsx
+++ b/static/p9.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t xml:space="preserve">DOMESTIC TAXES DEPARTMENT</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">DATE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/1/2020</t>
   </si>
 </sst>
 </file>
@@ -608,9 +611,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -624,7 +627,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5427720" y="114480"/>
-          <a:ext cx="2764800" cy="646920"/>
+          <a:ext cx="2763720" cy="646560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -646,8 +649,8 @@
   </sheetPr>
   <dimension ref="B6:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C48" activeCellId="0" sqref="C48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -658,7 +661,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.99"/>
@@ -1498,8 +1501,8 @@
       <c r="B47" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="41" t="n">
-        <v>43814</v>
+      <c r="C47" s="41" t="s">
+        <v>67</v>
       </c>
       <c r="D47" s="40"/>
       <c r="E47" s="40"/>

</xml_diff>

<commit_message>
Insert borders again to ensure they remain when the program runs
For some reason there were no borders and I didn't want to start
inserting them using the program as that is more code.
</commit_message>
<xml_diff>
--- a/static/p9.xlsx
+++ b/static/p9.xlsx
@@ -236,17 +236,16 @@
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="\ * #,##0.00\ ;\ * \(#,##0.00\);\ * \-#\ ;\ @\ "/>
+    <numFmt numFmtId="167" formatCode="\ * #,##0\ ;\ * \(#,##0\);\ * \-#\ ;\ @\ "/>
     <numFmt numFmtId="168" formatCode="#,##0"/>
     <numFmt numFmtId="169" formatCode="D\-MMM\-YY"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -260,6 +259,83 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -268,50 +344,102 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="17">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -391,8 +519,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="thin"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -418,21 +574,72 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,7 +647,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,115 +655,115 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -564,7 +771,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -572,7 +783,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -580,23 +791,100 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -611,9 +899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>65520</xdr:colOff>
+      <xdr:colOff>65160</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -627,7 +915,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5427720" y="114480"/>
-          <a:ext cx="2763720" cy="646560"/>
+          <a:ext cx="2763360" cy="646200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -649,8 +937,8 @@
   </sheetPr>
   <dimension ref="B6:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -998,7 +1286,7 @@
       <c r="P26" s="35"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="36" t="s">
         <v>46</v>
       </c>
       <c r="C27" s="33"/>
@@ -1033,7 +1321,7 @@
       <c r="P27" s="35"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="36" t="s">
         <v>47</v>
       </c>
       <c r="C28" s="33"/>
@@ -1068,7 +1356,7 @@
       <c r="P28" s="35"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="36" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="33"/>
@@ -1103,7 +1391,7 @@
       <c r="P29" s="35"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="36" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="33"/>
@@ -1138,7 +1426,7 @@
       <c r="P30" s="35"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="36" t="s">
         <v>50</v>
       </c>
       <c r="C31" s="33"/>
@@ -1173,7 +1461,7 @@
       <c r="P31" s="35"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="36" t="s">
         <v>51</v>
       </c>
       <c r="C32" s="33"/>
@@ -1208,7 +1496,7 @@
       <c r="P32" s="35"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="36" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="33"/>
@@ -1243,7 +1531,7 @@
       <c r="P33" s="35"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="36" t="s">
         <v>53</v>
       </c>
       <c r="C34" s="33"/>
@@ -1278,7 +1566,7 @@
       <c r="P34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="36" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="33"/>
@@ -1313,7 +1601,7 @@
       <c r="P35" s="35"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="33"/>
@@ -1348,7 +1636,7 @@
       <c r="P36" s="35"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="36" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="33"/>
@@ -1382,8 +1670,8 @@
       </c>
       <c r="P37" s="35"/>
     </row>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="36" t="s">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="37" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="33" t="n">
@@ -1422,23 +1710,23 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I40" s="38" t="s">
+      <c r="I40" s="39" t="s">
         <v>58</v>
       </c>
       <c r="K40" s="35" t="n">
@@ -1452,10 +1740,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="38" t="s">
+      <c r="B42" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="39" t="n">
+      <c r="E42" s="40" t="n">
         <f aca="false">L38</f>
         <v>0</v>
       </c>
@@ -1467,7 +1755,7 @@
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="40"/>
+      <c r="F44" s="41"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
@@ -1475,12 +1763,12 @@
       <c r="B45" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="40" t="s">
+      <c r="C45" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
@@ -1488,12 +1776,12 @@
       <c r="B46" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="40" t="s">
+      <c r="C46" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="D46" s="40"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
@@ -1501,12 +1789,12 @@
       <c r="B47" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C47" s="41" t="s">
+      <c r="C47" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
     </row>

</xml_diff>

<commit_message>
Change the year to 2022
</commit_message>
<xml_diff>
--- a/static/p9.xlsx
+++ b/static/p9.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">DOMESTIC TAXES DEPARTMENT</t>
   </si>
   <si>
-    <t xml:space="preserve">                       TAX DEDUCTION CARD YEAR…2021…………</t>
+    <t xml:space="preserve">                       TAX DEDUCTION CARD YEAR…2022…………</t>
   </si>
   <si>
     <t xml:space="preserve">P9A</t>
@@ -236,16 +236,17 @@
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="\ * #,##0.00\ ;\ * \(#,##0.00\);\ * \-#\ ;\ @\ "/>
-    <numFmt numFmtId="167" formatCode="\ * #,##0\ ;\ * \(#,##0\);\ * \-#\ ;\ @\ "/>
+    <numFmt numFmtId="166" formatCode="* #,##0.00\ ;* \(#,##0.00\);* \-#\ ;@\ "/>
+    <numFmt numFmtId="167" formatCode="* #,##0\ ;* \(#,##0\);* \-#\ ;@\ "/>
     <numFmt numFmtId="168" formatCode="#,##0"/>
-    <numFmt numFmtId="169" formatCode="D\-MMM\-YY"/>
+    <numFmt numFmtId="169" formatCode="d\-mmm\-yy"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -264,182 +265,53 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -548,7 +420,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -574,72 +446,21 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -647,7 +468,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -655,115 +476,115 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -771,11 +592,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -783,7 +604,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -791,100 +612,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -899,9 +643,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>64800</xdr:colOff>
+      <xdr:colOff>64440</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>112680</xdr:rowOff>
+      <xdr:rowOff>112320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -915,12 +659,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5427720" y="114480"/>
-          <a:ext cx="2763000" cy="645840"/>
+          <a:ext cx="2762640" cy="645480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
+        <a:ln w="0">
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
@@ -931,26 +675,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B6:P47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.57"/>
@@ -958,9 +700,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="16" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1810,8 +1550,8 @@
     <mergeCell ref="K24:K25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="0.479861111111111" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="59" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="0.479861111111111" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="59" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Change files to point to 2023
</commit_message>
<xml_diff>
--- a/static/p9.xlsx
+++ b/static/p9.xlsx
@@ -230,7 +230,7 @@
     <t>15/1/2020</t>
   </si>
   <si>
-    <t xml:space="preserve">                       TAX DEDUCTION CARD YEAR…2022…………</t>
+    <t xml:space="preserve">                       TAX DEDUCTION CARD YEAR…2023…………</t>
   </si>
 </sst>
 </file>
@@ -498,24 +498,6 @@
   </cellStyleXfs>
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -573,6 +555,24 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -994,43 +994,43 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="B6" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
     </row>
     <row r="7" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1038,29 +1038,29 @@
       <c r="B10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J10" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="M10" s="42"/>
+      <c r="N10" s="42"/>
     </row>
     <row r="11" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="8"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
+      <c r="D11" s="2"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="2:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1070,696 +1070,696 @@
       <c r="J14" t="s">
         <v>8</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="42"/>
     </row>
     <row r="19" spans="2:16" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="13" t="s">
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="L19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="M19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="N19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="18" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="O20" s="19"/>
+      <c r="O20" s="13"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="19"/>
+      <c r="O21" s="13"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B22" s="22"/>
-      <c r="C22" s="23" t="s">
+      <c r="B22" s="16"/>
+      <c r="C22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="26" t="s">
+      <c r="I22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="23" t="s">
+      <c r="K22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="L22" s="23" t="s">
+      <c r="L22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="M22" s="23" t="s">
+      <c r="M22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="N22" s="23" t="s">
+      <c r="N22" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="O22" s="26" t="s">
+      <c r="O22" s="20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
-      <c r="C23" s="11" t="s">
+      <c r="B23" s="4"/>
+      <c r="C23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="11" t="s">
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L23" s="11" t="s">
+      <c r="L23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M23" s="11" t="s">
+      <c r="M23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N23" s="11" t="s">
+      <c r="N23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="O23" s="11" t="s">
+      <c r="O23" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="27" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I24" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K24" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
     </row>
     <row r="25" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="30" t="s">
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="31" t="s">
+      <c r="H25" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="I25" s="32" t="s">
+      <c r="I25" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
-      <c r="O25" s="29"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34">
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28">
         <f t="shared" ref="F26:F37" si="0">C26</f>
         <v>0</v>
       </c>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34">
-        <v>0</v>
-      </c>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34">
+      <c r="G26" s="28"/>
+      <c r="H26" s="28">
+        <v>0</v>
+      </c>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28">
         <f t="shared" ref="K26:K38" si="1">H26</f>
         <v>0</v>
       </c>
-      <c r="L26" s="34">
+      <c r="L26" s="28">
         <f t="shared" ref="L26:L37" si="2">F26-K26</f>
         <v>0</v>
       </c>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34">
+      <c r="M26" s="28"/>
+      <c r="N26" s="28">
         <v>2400</v>
       </c>
-      <c r="O26" s="35">
+      <c r="O26" s="29">
         <f t="shared" ref="O26:O37" si="3">+M26-N26</f>
         <v>-2400</v>
       </c>
-      <c r="P26" s="36"/>
+      <c r="P26" s="30"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34">
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34">
-        <v>0</v>
-      </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34">
+      <c r="G27" s="28"/>
+      <c r="H27" s="28">
+        <v>0</v>
+      </c>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L27" s="34">
+      <c r="L27" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34">
+      <c r="M27" s="28"/>
+      <c r="N27" s="28">
         <v>2400</v>
       </c>
-      <c r="O27" s="35">
+      <c r="O27" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P27" s="36"/>
+      <c r="P27" s="30"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34">
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34">
-        <v>0</v>
-      </c>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34">
+      <c r="G28" s="28"/>
+      <c r="H28" s="28">
+        <v>0</v>
+      </c>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L28" s="34">
+      <c r="L28" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34">
+      <c r="M28" s="28"/>
+      <c r="N28" s="28">
         <v>2400</v>
       </c>
-      <c r="O28" s="35">
+      <c r="O28" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P28" s="36"/>
+      <c r="P28" s="30"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34">
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="34"/>
-      <c r="H29" s="34">
-        <v>0</v>
-      </c>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34">
+      <c r="G29" s="28"/>
+      <c r="H29" s="28">
+        <v>0</v>
+      </c>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L29" s="34">
+      <c r="L29" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M29" s="34"/>
-      <c r="N29" s="34">
+      <c r="M29" s="28"/>
+      <c r="N29" s="28">
         <v>2400</v>
       </c>
-      <c r="O29" s="35">
+      <c r="O29" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P29" s="36"/>
+      <c r="P29" s="30"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34">
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34">
-        <v>0</v>
-      </c>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34">
+      <c r="G30" s="28"/>
+      <c r="H30" s="28">
+        <v>0</v>
+      </c>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L30" s="34">
+      <c r="L30" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34">
+      <c r="M30" s="28"/>
+      <c r="N30" s="28">
         <v>2400</v>
       </c>
-      <c r="O30" s="35">
+      <c r="O30" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P30" s="36"/>
+      <c r="P30" s="30"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34">
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34">
-        <v>0</v>
-      </c>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34">
+      <c r="G31" s="28"/>
+      <c r="H31" s="28">
+        <v>0</v>
+      </c>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L31" s="34">
+      <c r="L31" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34">
+      <c r="M31" s="28"/>
+      <c r="N31" s="28">
         <v>2400</v>
       </c>
-      <c r="O31" s="35">
+      <c r="O31" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P31" s="36"/>
+      <c r="P31" s="30"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34">
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34">
-        <v>0</v>
-      </c>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34">
+      <c r="G32" s="28"/>
+      <c r="H32" s="28">
+        <v>0</v>
+      </c>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L32" s="34">
+      <c r="L32" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34">
+      <c r="M32" s="28"/>
+      <c r="N32" s="28">
         <v>2400</v>
       </c>
-      <c r="O32" s="35">
+      <c r="O32" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P32" s="36"/>
+      <c r="P32" s="30"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34">
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34">
-        <v>0</v>
-      </c>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-      <c r="K33" s="34">
+      <c r="G33" s="28"/>
+      <c r="H33" s="28">
+        <v>0</v>
+      </c>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L33" s="34">
+      <c r="L33" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34">
+      <c r="M33" s="28"/>
+      <c r="N33" s="28">
         <v>2400</v>
       </c>
-      <c r="O33" s="35">
+      <c r="O33" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P33" s="36"/>
+      <c r="P33" s="30"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34">
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34">
-        <v>0</v>
-      </c>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34">
+      <c r="G34" s="28"/>
+      <c r="H34" s="28">
+        <v>0</v>
+      </c>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L34" s="34">
+      <c r="L34" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34">
+      <c r="M34" s="28"/>
+      <c r="N34" s="28">
         <v>2400</v>
       </c>
-      <c r="O34" s="35">
+      <c r="O34" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P34" s="36"/>
+      <c r="P34" s="30"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34">
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34">
-        <v>0</v>
-      </c>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="34">
+      <c r="G35" s="28"/>
+      <c r="H35" s="28">
+        <v>0</v>
+      </c>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L35" s="34">
+      <c r="L35" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M35" s="34"/>
-      <c r="N35" s="34">
+      <c r="M35" s="28"/>
+      <c r="N35" s="28">
         <v>2400</v>
       </c>
-      <c r="O35" s="35">
+      <c r="O35" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P35" s="36"/>
+      <c r="P35" s="30"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34">
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="34"/>
-      <c r="H36" s="34">
-        <v>0</v>
-      </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34">
+      <c r="G36" s="28"/>
+      <c r="H36" s="28">
+        <v>0</v>
+      </c>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L36" s="34">
+      <c r="L36" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34">
+      <c r="M36" s="28"/>
+      <c r="N36" s="28">
         <v>2400</v>
       </c>
-      <c r="O36" s="35">
+      <c r="O36" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P36" s="36"/>
+      <c r="P36" s="30"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34">
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G37" s="34"/>
-      <c r="H37" s="34">
-        <v>0</v>
-      </c>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34">
+      <c r="G37" s="28"/>
+      <c r="H37" s="28">
+        <v>0</v>
+      </c>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L37" s="34">
+      <c r="L37" s="28">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34">
+      <c r="M37" s="28"/>
+      <c r="N37" s="28">
         <v>2400</v>
       </c>
-      <c r="O37" s="35">
+      <c r="O37" s="29">
         <f t="shared" si="3"/>
         <v>-2400</v>
       </c>
-      <c r="P37" s="36"/>
+      <c r="P37" s="30"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="34">
+      <c r="C38" s="28">
         <f>SUM(C26:C37)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34">
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28">
         <f>SUM(F26:F37)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34">
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L38" s="34">
+      <c r="L38" s="28">
         <f>SUM(L26:L37)</f>
         <v>0</v>
       </c>
-      <c r="M38" s="34">
+      <c r="M38" s="28">
         <f>SUM(M26:M37)</f>
         <v>0</v>
       </c>
-      <c r="N38" s="34">
+      <c r="N38" s="28">
         <f>SUM(N26:N37)</f>
         <v>28800</v>
       </c>
-      <c r="O38" s="34">
+      <c r="O38" s="28">
         <f>SUM(O26:O37)</f>
         <v>-28800</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B39" s="39"/>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-      <c r="K39" s="39"/>
-      <c r="L39" s="39"/>
-      <c r="M39" s="39"/>
-      <c r="N39" s="39"/>
-      <c r="O39" s="39"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I40" s="40" t="s">
+      <c r="I40" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="K40" s="36">
+      <c r="K40" s="30">
         <f>O38</f>
         <v>-28800</v>
       </c>
@@ -1770,63 +1770,63 @@
       </c>
     </row>
     <row r="42" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="40" t="s">
+      <c r="B42" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="41">
+      <c r="E42" s="35">
         <f>L38</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="8"/>
-      <c r="C44" s="7" t="s">
+      <c r="B44" s="2"/>
+      <c r="C44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
     </row>
     <row r="45" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
     </row>
     <row r="46" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="42" t="s">
+      <c r="C46" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
     </row>
     <row r="47" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="43" t="s">
+      <c r="C47" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>